<commit_message>
presentation notebook to fifth example
</commit_message>
<xml_diff>
--- a/tests/portfolio_small3.xlsx
+++ b/tests/portfolio_small3.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20396"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Programming\python\PyProtolinc\tests\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04DA8304-BA48-4CF6-A289-6767E0924A57}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-420" windowWidth="29040" windowHeight="15840" tabRatio="500"/>
+    <workbookView xWindow="-28920" yWindow="-420" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -78,18 +84,14 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.00000000"/>
+  </numFmts>
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
@@ -118,7 +120,7 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -425,32 +427,32 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:L10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5:H19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.7109375" customWidth="1"/>
-    <col min="3" max="3" width="15.140625" customWidth="1"/>
-    <col min="4" max="4" width="22.7109375" customWidth="1"/>
-    <col min="5" max="5" width="13.7109375" customWidth="1"/>
-    <col min="6" max="6" width="16.85546875" customWidth="1"/>
-    <col min="8" max="8" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.6640625" customWidth="1"/>
+    <col min="3" max="3" width="15.109375" customWidth="1"/>
+    <col min="4" max="4" width="22.6640625" customWidth="1"/>
+    <col min="5" max="5" width="13.6640625" customWidth="1"/>
+    <col min="6" max="6" width="16.88671875" customWidth="1"/>
+    <col min="8" max="8" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -488,7 +490,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:12">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>44561</v>
       </c>
@@ -519,9 +521,11 @@
       <c r="K2">
         <v>0</v>
       </c>
-      <c r="L2" s="2"/>
+      <c r="L2" s="1">
+        <v>44592</v>
+      </c>
     </row>
-    <row r="3" spans="1:12">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>44561</v>
       </c>
@@ -552,9 +556,11 @@
       <c r="K3">
         <v>0</v>
       </c>
-      <c r="L3" s="2"/>
+      <c r="L3" s="1">
+        <v>45077</v>
+      </c>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>44561</v>
       </c>
@@ -585,7 +591,12 @@
       <c r="K4">
         <v>0</v>
       </c>
-      <c r="L4" s="2"/>
+      <c r="L4" s="1">
+        <v>38631</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="E10" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>